<commit_message>
Mod by yxq @20171127
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/marg.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/marg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="19104" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>各环节时间参数(如图)</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>135分钟</t>
+  </si>
+  <si>
+    <t>用户输入</t>
   </si>
   <si>
     <t>上车装货时间</t>
@@ -89,10 +92,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -112,8 +115,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,93 +137,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,6 +153,79 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -235,21 +236,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,187 +267,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,41 +476,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -530,8 +503,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,8 +527,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +548,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -578,10 +581,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -590,133 +593,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1078,10 +1081,10 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="67.8333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.83333333333333" style="1"/>
@@ -1106,95 +1109,113 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1212,7 +1233,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1229,7 +1250,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>